<commit_message>
formulu labojumi un izmēģinājumi
</commit_message>
<xml_diff>
--- a/trip_costs.xlsx
+++ b/trip_costs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,62 @@
         <v>39.3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>556</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="D3" t="n">
+        <v>112.59</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>420</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>88.87</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>420</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>19.32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>420</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>28.98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>